<commit_message>
excel et renommation SEM
</commit_message>
<xml_diff>
--- a/Synthèse-Experiences/ExperimentsMAJ13juillet.xlsx
+++ b/Synthèse-Experiences/ExperimentsMAJ13juillet.xlsx
@@ -990,7 +990,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1252,9 +1252,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1265,6 +1262,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1292,10 +1295,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1318,7 +1321,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="81">
     <dxf>
       <font>
         <b val="0"/>
@@ -1335,6 +1338,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1349,33 +1353,13 @@
         <right style="thin">
           <color rgb="FFBBBBAD"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color rgb="FFBBBBAD"/>
+        </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
@@ -1456,6 +1440,64 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFBBBBAD"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFBBBBAD"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FFBBBBAD"/>
@@ -3406,79 +3448,6 @@
         <bottom style="thin">
           <color rgb="FFBBBBAD"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFBBBBAD"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFBBBBAD"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFBBBBAD"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFBBBBAD"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFBBBBAD"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3662,79 +3631,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:AG60" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:AG60" dataDxfId="80">
   <autoFilter ref="A3:AG60"/>
   <sortState ref="A4:AF33">
     <sortCondition ref="D3:D33"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="27" name="# Exp" totalsRowLabel="Total" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="32" name="Position U" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="31" name="Position V" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="1" name="Date" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="2" name="Sample" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="3" name="Coating" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="4" name="Coating thickness" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="5" name="Design" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="6" name="Design dose factor" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="7" name="Beam" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="8" name="Loop factor" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="9" name="Current (pA)" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="10" name="Dot         pC" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="11" name="Line μC/cm" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="12" name="Area μC/cm^2" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="13" name="Area/Line step size (𝝁m)" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="14" name="Min Dot DF" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="15" name="Total11 charge pC" dataDxfId="46" totalsRowDxfId="45">
+    <tableColumn id="27" name="# Exp" totalsRowLabel="Total" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="32" name="Position U" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="31" name="Position V" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="2" name="Sample" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="3" name="Coating" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="4" name="Coating thickness" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" name="Design" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="6" name="Design dose factor" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="7" name="Beam" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="8" name="Loop factor" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="9" name="Current (pA)" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="10" name="Dot         pC" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="11" name="Line μC/cm" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="12" name="Area μC/cm^2" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="13" name="Area/Line step size (𝝁m)" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="14" name="Min Dot DF" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="15" name="Total11 charge pC" dataDxfId="47" totalsRowDxfId="46">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Max Dot DF" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="17" name="Total12 charge pC" dataDxfId="42" totalsRowDxfId="41">
+    <tableColumn id="16" name="Max Dot DF" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="17" name="Total12 charge pC" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Min Line DF" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="19" name="Total21 charge µC" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="18" name="Min Line DF" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="19" name="Total21 charge µC" dataDxfId="39" totalsRowDxfId="38">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Max Line DF" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="21" name="Total22 charge µC" dataDxfId="34" totalsRowDxfId="33">
+    <tableColumn id="20" name="Max Line DF" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="21" name="Total22 charge µC" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Min Area DF" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="23" name="Total31 charge μC" dataDxfId="30" totalsRowDxfId="29">
+    <tableColumn id="22" name="Min Area DF" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="23" name="Total31 charge μC" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Max Area DF" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="25" name="Totale charge32 μC" dataDxfId="26" totalsRowDxfId="25">
+    <tableColumn id="24" name="Max Area DF" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="25" name="Totale charge32 μC" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Total hole size" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="28" name="Step between dots" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="29" name="Charge" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="30" name="Results" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="33" name="SEM (upside down)" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="26" name="Total hole size" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="28" name="Step between dots" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="29" name="Charge" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="30" name="Results" totalsRowFunction="count" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="33" name="SEM (upside down)" dataDxfId="17" totalsRowDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:M15" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:M15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:M15"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Beam" dataDxfId="14"/>
-    <tableColumn id="14" name="Design" dataDxfId="13"/>
-    <tableColumn id="2" name="loops" dataDxfId="12"/>
-    <tableColumn id="3" name="min charge for dot piercing (pC)" dataDxfId="11"/>
-    <tableColumn id="4" name="min charge for line piercing (μC)" dataDxfId="10"/>
-    <tableColumn id="5" name="min charge for area piercing (μC)" dataDxfId="9"/>
-    <tableColumn id="6" name="Comments" dataDxfId="8"/>
-    <tableColumn id="7" name="Colonne7" dataDxfId="7"/>
-    <tableColumn id="8" name="Colonne8" dataDxfId="6"/>
-    <tableColumn id="9" name="Colonne9" dataDxfId="5"/>
-    <tableColumn id="10" name="Colonne10" dataDxfId="4"/>
-    <tableColumn id="11" name="Colonne11" dataDxfId="3"/>
-    <tableColumn id="12" name="Colonne12" dataDxfId="2"/>
+    <tableColumn id="1" name="Beam" dataDxfId="13"/>
+    <tableColumn id="14" name="Design" dataDxfId="12"/>
+    <tableColumn id="2" name="loops" dataDxfId="11"/>
+    <tableColumn id="3" name="min charge for dot piercing (pC)" dataDxfId="10"/>
+    <tableColumn id="4" name="min charge for line piercing (μC)" dataDxfId="9"/>
+    <tableColumn id="5" name="min charge for area piercing (μC)" dataDxfId="8"/>
+    <tableColumn id="6" name="Comments" dataDxfId="7"/>
+    <tableColumn id="7" name="Colonne7" dataDxfId="6"/>
+    <tableColumn id="8" name="Colonne8" dataDxfId="5"/>
+    <tableColumn id="9" name="Colonne9" dataDxfId="4"/>
+    <tableColumn id="10" name="Colonne10" dataDxfId="3"/>
+    <tableColumn id="11" name="Colonne11" dataDxfId="2"/>
+    <tableColumn id="12" name="Colonne12" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4065,10 +4034,10 @@
   <dimension ref="A1:AG60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="X24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG28" sqref="AG28"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56:AG56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4111,32 +4080,32 @@
       <c r="J1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="98" t="s">
+      <c r="K1" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="98"/>
+      <c r="L1" s="99"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="37"/>
-      <c r="Q1" s="100" t="s">
+      <c r="Q1" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="101" t="s">
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="101"/>
+      <c r="U1" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="102" t="s">
+      <c r="V1" s="102"/>
+      <c r="W1" s="102"/>
+      <c r="X1" s="102"/>
+      <c r="Y1" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
       <c r="AD1" s="49" t="s">
         <v>68</v>
       </c>
@@ -4144,41 +4113,41 @@
     </row>
     <row r="2" spans="1:33" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H2" s="60"/>
-      <c r="M2" s="103" t="s">
+      <c r="M2" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
       <c r="P2" s="37"/>
-      <c r="Q2" s="104" t="s">
+      <c r="Q2" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104" t="s">
+      <c r="R2" s="105"/>
+      <c r="S2" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="104"/>
-      <c r="U2" s="105" t="s">
+      <c r="T2" s="105"/>
+      <c r="U2" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105" t="s">
+      <c r="V2" s="106"/>
+      <c r="W2" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="106" t="s">
+      <c r="X2" s="106"/>
+      <c r="Y2" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="106"/>
-      <c r="AA2" s="106" t="s">
+      <c r="Z2" s="107"/>
+      <c r="AA2" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="106"/>
-      <c r="AC2" s="99" t="s">
+      <c r="AB2" s="107"/>
+      <c r="AC2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="99"/>
-      <c r="AE2" s="99"/>
+      <c r="AD2" s="100"/>
+      <c r="AE2" s="100"/>
     </row>
     <row r="3" spans="1:33" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
@@ -4277,7 +4246,7 @@
       <c r="AF3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AG3" s="108" t="s">
+      <c r="AG3" s="98" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4362,7 +4331,7 @@
       <c r="AD4" s="13"/>
       <c r="AE4" s="13"/>
       <c r="AF4" s="15"/>
-      <c r="AG4" s="107"/>
+      <c r="AG4" s="97"/>
     </row>
     <row r="5" spans="1:33" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="34">
@@ -4447,7 +4416,7 @@
       <c r="AF5" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AG5" s="107"/>
+      <c r="AG5" s="97"/>
     </row>
     <row r="6" spans="1:33" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="32">
@@ -4531,7 +4500,7 @@
       <c r="AF6" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="AG6" s="107"/>
+      <c r="AG6" s="97"/>
     </row>
     <row r="7" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="34">
@@ -4616,7 +4585,7 @@
       <c r="AF7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AG7" s="107"/>
+      <c r="AG7" s="97"/>
     </row>
     <row r="8" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="32">
@@ -4701,7 +4670,7 @@
       <c r="AD8" s="13"/>
       <c r="AE8" s="13"/>
       <c r="AF8" s="15"/>
-      <c r="AG8" s="107"/>
+      <c r="AG8" s="97"/>
     </row>
     <row r="9" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="32">
@@ -4790,7 +4759,7 @@
       <c r="AF9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AG9" s="107"/>
+      <c r="AG9" s="97"/>
     </row>
     <row r="10" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
@@ -4879,7 +4848,7 @@
       <c r="AF10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="107"/>
+      <c r="AG10" s="97"/>
     </row>
     <row r="11" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="32">
@@ -4970,7 +4939,7 @@
       <c r="AF11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AG11" s="107"/>
+      <c r="AG11" s="97"/>
     </row>
     <row r="12" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
@@ -5063,7 +5032,7 @@
         <v>70</v>
       </c>
       <c r="AF12" s="15"/>
-      <c r="AG12" s="107"/>
+      <c r="AG12" s="97"/>
     </row>
     <row r="13" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
@@ -5150,7 +5119,7 @@
       <c r="AF13" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="AG13" s="107"/>
+      <c r="AG13" s="97"/>
     </row>
     <row r="14" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="32">
@@ -5241,7 +5210,7 @@
       <c r="AD14" s="15"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15"/>
-      <c r="AG14" s="107"/>
+      <c r="AG14" s="97"/>
     </row>
     <row r="15" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
@@ -5330,7 +5299,7 @@
       </c>
       <c r="AE15" s="48"/>
       <c r="AF15" s="15"/>
-      <c r="AG15" s="107"/>
+      <c r="AG15" s="97"/>
     </row>
     <row r="16" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
@@ -5419,7 +5388,7 @@
       </c>
       <c r="AE16" s="48"/>
       <c r="AF16" s="15"/>
-      <c r="AG16" s="107"/>
+      <c r="AG16" s="97"/>
     </row>
     <row r="17" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="32">
@@ -5516,7 +5485,7 @@
       <c r="AF17" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="AG17" s="107"/>
+      <c r="AG17" s="97"/>
     </row>
     <row r="18" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="32">
@@ -5613,7 +5582,7 @@
       <c r="AF18" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="AG18" s="107"/>
+      <c r="AG18" s="97"/>
     </row>
     <row r="19" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="32">
@@ -5702,7 +5671,7 @@
       <c r="AD19" s="58"/>
       <c r="AE19" s="58"/>
       <c r="AF19" s="58"/>
-      <c r="AG19" s="107"/>
+      <c r="AG19" s="97"/>
     </row>
     <row r="20" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
@@ -5795,7 +5764,7 @@
       <c r="AF20" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="AG20" s="107"/>
+      <c r="AG20" s="97"/>
     </row>
     <row r="21" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="32">
@@ -5880,7 +5849,7 @@
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
       <c r="AF21" s="15"/>
-      <c r="AG21" s="107"/>
+      <c r="AG21" s="97"/>
     </row>
     <row r="22" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
@@ -5967,7 +5936,7 @@
       <c r="AF22" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="AG22" s="107"/>
+      <c r="AG22" s="97"/>
     </row>
     <row r="23" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
@@ -6053,7 +6022,7 @@
       <c r="AD23" s="15"/>
       <c r="AE23" s="15"/>
       <c r="AF23" s="15"/>
-      <c r="AG23" s="107"/>
+      <c r="AG23" s="97"/>
     </row>
     <row r="24" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="32">
@@ -6063,7 +6032,6 @@
         <v>99</v>
       </c>
       <c r="C24" s="73">
-        <f>C23-0.001</f>
         <v>2.738</v>
       </c>
       <c r="D24" s="65">
@@ -6140,7 +6108,7 @@
       <c r="AD24" s="15"/>
       <c r="AE24" s="15"/>
       <c r="AF24" s="15"/>
-      <c r="AG24" s="107"/>
+      <c r="AG24" s="97"/>
     </row>
     <row r="25" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="32">
@@ -6150,7 +6118,6 @@
         <v>99</v>
       </c>
       <c r="C25" s="73">
-        <f t="shared" ref="C25:C36" si="1">C24-0.001</f>
         <v>2.7370000000000001</v>
       </c>
       <c r="D25" s="65">
@@ -6226,7 +6193,7 @@
       <c r="AC25" s="15"/>
       <c r="AD25" s="15"/>
       <c r="AE25" s="15"/>
-      <c r="AG25" s="107"/>
+      <c r="AG25" s="97"/>
     </row>
     <row r="26" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A26" s="32">
@@ -6314,7 +6281,7 @@
       <c r="AF26" t="s">
         <v>105</v>
       </c>
-      <c r="AG26" s="107"/>
+      <c r="AG26" s="97"/>
     </row>
     <row r="27" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="32">
@@ -6324,7 +6291,6 @@
         <v>99</v>
       </c>
       <c r="C27" s="73">
-        <f t="shared" si="1"/>
         <v>2.7360000000000002</v>
       </c>
       <c r="D27" s="65">
@@ -6403,7 +6369,7 @@
       <c r="AD27" s="15"/>
       <c r="AE27" s="15"/>
       <c r="AF27" s="15"/>
-      <c r="AG27" s="107"/>
+      <c r="AG27" s="97"/>
     </row>
     <row r="28" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="32">
@@ -6413,7 +6379,6 @@
         <v>99</v>
       </c>
       <c r="C28" s="73">
-        <f t="shared" si="1"/>
         <v>2.7350000000000003</v>
       </c>
       <c r="D28" s="65">
@@ -6494,7 +6459,7 @@
       <c r="AF28" t="s">
         <v>104</v>
       </c>
-      <c r="AG28" s="107"/>
+      <c r="AG28" s="97"/>
     </row>
     <row r="29" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="32">
@@ -6504,7 +6469,6 @@
         <v>99</v>
       </c>
       <c r="C29" s="73">
-        <f t="shared" si="1"/>
         <v>2.7340000000000004</v>
       </c>
       <c r="D29" s="65">
@@ -6581,7 +6545,7 @@
       <c r="AD29" s="15"/>
       <c r="AE29" s="15"/>
       <c r="AF29" s="15"/>
-      <c r="AG29" s="107"/>
+      <c r="AG29" s="97"/>
     </row>
     <row r="30" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="33">
@@ -6591,7 +6555,6 @@
         <v>99</v>
       </c>
       <c r="C30" s="73">
-        <f t="shared" si="1"/>
         <v>2.7330000000000005</v>
       </c>
       <c r="D30" s="65">
@@ -6668,7 +6631,7 @@
       <c r="AD30" s="15"/>
       <c r="AE30" s="15"/>
       <c r="AF30" s="15"/>
-      <c r="AG30" s="107"/>
+      <c r="AG30" s="97"/>
     </row>
     <row r="31" spans="1:33" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A31" s="33">
@@ -6678,7 +6641,6 @@
         <v>99</v>
       </c>
       <c r="C31" s="73">
-        <f t="shared" si="1"/>
         <v>2.7320000000000007</v>
       </c>
       <c r="D31" s="65">
@@ -6755,7 +6717,7 @@
       <c r="AD31" s="28"/>
       <c r="AE31" s="28"/>
       <c r="AF31" s="28"/>
-      <c r="AG31" s="107"/>
+      <c r="AG31" s="97"/>
     </row>
     <row r="32" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="33">
@@ -6765,7 +6727,6 @@
         <v>99</v>
       </c>
       <c r="C32" s="73">
-        <f t="shared" si="1"/>
         <v>2.7310000000000008</v>
       </c>
       <c r="D32" s="65">
@@ -6841,7 +6802,7 @@
       <c r="AC32" s="28"/>
       <c r="AD32" s="28"/>
       <c r="AE32" s="28"/>
-      <c r="AG32" s="107"/>
+      <c r="AG32" s="97"/>
     </row>
     <row r="33" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="33">
@@ -6851,7 +6812,6 @@
         <v>99</v>
       </c>
       <c r="C33" s="73">
-        <f t="shared" si="1"/>
         <v>2.7300000000000009</v>
       </c>
       <c r="D33" s="65">
@@ -6928,7 +6888,7 @@
       <c r="AD33" s="28"/>
       <c r="AE33" s="28"/>
       <c r="AF33" s="28"/>
-      <c r="AG33" s="107"/>
+      <c r="AG33" s="97"/>
     </row>
     <row r="34" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="33">
@@ -6938,7 +6898,6 @@
         <v>99</v>
       </c>
       <c r="C34" s="73">
-        <f t="shared" si="1"/>
         <v>2.729000000000001</v>
       </c>
       <c r="D34" s="65">
@@ -7015,7 +6974,7 @@
       <c r="AD34" s="28"/>
       <c r="AE34" s="28"/>
       <c r="AF34" s="28"/>
-      <c r="AG34" s="107"/>
+      <c r="AG34" s="97"/>
     </row>
     <row r="35" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="33">
@@ -7025,7 +6984,6 @@
         <v>99</v>
       </c>
       <c r="C35" s="73">
-        <f t="shared" si="1"/>
         <v>2.7280000000000011</v>
       </c>
       <c r="D35" s="65">
@@ -7102,7 +7060,7 @@
       <c r="AD35" s="28"/>
       <c r="AE35" s="28"/>
       <c r="AF35" s="28"/>
-      <c r="AG35" s="107"/>
+      <c r="AG35" s="97"/>
     </row>
     <row r="36" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="33">
@@ -7112,7 +7070,6 @@
         <v>99</v>
       </c>
       <c r="C36" s="73">
-        <f t="shared" si="1"/>
         <v>2.7270000000000012</v>
       </c>
       <c r="D36" s="65">
@@ -7189,7 +7146,7 @@
       <c r="AD36" s="28"/>
       <c r="AE36" s="28"/>
       <c r="AF36" s="28"/>
-      <c r="AG36" s="107"/>
+      <c r="AG36" s="97"/>
     </row>
     <row r="37" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="33">
@@ -7275,11 +7232,10 @@
       <c r="AD37" s="28"/>
       <c r="AE37" s="28"/>
       <c r="AF37" s="28"/>
-      <c r="AG37" s="107"/>
+      <c r="AG37" s="97"/>
     </row>
     <row r="38" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="33">
-        <f>A37+1</f>
+      <c r="A38" s="108">
         <v>36</v>
       </c>
       <c r="B38" s="80">
@@ -7355,18 +7311,16 @@
       <c r="AD38" s="28"/>
       <c r="AE38" s="28"/>
       <c r="AF38" s="28"/>
-      <c r="AG38" s="107"/>
+      <c r="AG38" s="97"/>
     </row>
     <row r="39" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="33">
-        <f t="shared" ref="A39:A60" si="2">A38+1</f>
+      <c r="A39" s="108">
         <v>37</v>
       </c>
       <c r="B39" s="80">
         <v>2.7309999999999999</v>
       </c>
       <c r="C39" s="74">
-        <f>C38+0.001</f>
         <v>2.7130000000000001</v>
       </c>
       <c r="D39" s="68" t="s">
@@ -7436,18 +7390,16 @@
       <c r="AD39" s="28"/>
       <c r="AE39" s="28"/>
       <c r="AF39" s="28"/>
-      <c r="AG39" s="107"/>
+      <c r="AG39" s="97"/>
     </row>
     <row r="40" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="33">
-        <f t="shared" si="2"/>
+      <c r="A40" s="108">
         <v>38</v>
       </c>
       <c r="B40" s="80">
         <v>2.7309999999999999</v>
       </c>
       <c r="C40" s="74">
-        <f t="shared" ref="C40:C43" si="3">C39+0.001</f>
         <v>2.714</v>
       </c>
       <c r="D40" s="68" t="s">
@@ -7517,18 +7469,16 @@
       <c r="AD40" s="28"/>
       <c r="AE40" s="28"/>
       <c r="AF40" s="15"/>
-      <c r="AG40" s="107"/>
+      <c r="AG40" s="97"/>
     </row>
     <row r="41" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="33">
-        <f t="shared" si="2"/>
+      <c r="A41" s="108">
         <v>39</v>
       </c>
       <c r="B41" s="80">
         <v>2.7309999999999999</v>
       </c>
       <c r="C41" s="74">
-        <f t="shared" si="3"/>
         <v>2.7149999999999999</v>
       </c>
       <c r="D41" s="68" t="s">
@@ -7598,18 +7548,16 @@
       <c r="AD41" s="92"/>
       <c r="AE41" s="92"/>
       <c r="AF41" s="15"/>
-      <c r="AG41" s="107"/>
+      <c r="AG41" s="97"/>
     </row>
     <row r="42" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="33">
-        <f t="shared" si="2"/>
+      <c r="A42" s="108">
         <v>40</v>
       </c>
       <c r="B42" s="80">
         <v>2.7309999999999999</v>
       </c>
       <c r="C42" s="74">
-        <f t="shared" si="3"/>
         <v>2.7159999999999997</v>
       </c>
       <c r="D42" s="68" t="s">
@@ -7679,18 +7627,16 @@
       <c r="AD42" s="92"/>
       <c r="AE42" s="92"/>
       <c r="AF42" s="15"/>
-      <c r="AG42" s="107"/>
+      <c r="AG42" s="97"/>
     </row>
     <row r="43" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="33">
-        <f t="shared" si="2"/>
+      <c r="A43" s="108">
         <v>41</v>
       </c>
       <c r="B43" s="80">
         <v>2.7309999999999999</v>
       </c>
       <c r="C43" s="74">
-        <f t="shared" si="3"/>
         <v>2.7169999999999996</v>
       </c>
       <c r="D43" s="68" t="s">
@@ -7760,18 +7706,16 @@
       <c r="AD43" s="92"/>
       <c r="AE43" s="92"/>
       <c r="AF43" s="15"/>
-      <c r="AG43" s="107"/>
+      <c r="AG43" s="97"/>
     </row>
     <row r="44" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="33">
-        <f t="shared" si="2"/>
+      <c r="A44" s="108">
         <v>42</v>
       </c>
       <c r="B44" s="80">
         <v>2.7320000000000002</v>
       </c>
       <c r="C44" s="74">
-        <f>C43</f>
         <v>2.7169999999999996</v>
       </c>
       <c r="D44" s="68" t="s">
@@ -7841,11 +7785,10 @@
       <c r="AD44" s="92"/>
       <c r="AE44" s="92"/>
       <c r="AF44" s="15"/>
-      <c r="AG44" s="107"/>
+      <c r="AG44" s="97"/>
     </row>
-    <row r="45" spans="1:33" s="97" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="93">
-        <f t="shared" si="2"/>
+    <row r="45" spans="1:33" s="96" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="108">
         <v>43</v>
       </c>
       <c r="B45" s="82"/>
@@ -7871,49 +7814,48 @@
       <c r="L45" s="87"/>
       <c r="M45" s="87"/>
       <c r="N45" s="87"/>
-      <c r="O45" s="94"/>
+      <c r="O45" s="93"/>
       <c r="P45" s="87"/>
       <c r="Q45" s="87"/>
-      <c r="R45" s="95">
+      <c r="R45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="S45" s="87"/>
-      <c r="T45" s="95">
+      <c r="T45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="U45" s="87"/>
-      <c r="V45" s="95">
+      <c r="V45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
       <c r="W45" s="87"/>
-      <c r="X45" s="95">
+      <c r="X45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
       <c r="Y45" s="87"/>
-      <c r="Z45" s="95">
+      <c r="Z45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AA45" s="87"/>
-      <c r="AB45" s="95">
+      <c r="AB45" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC45" s="87"/>
-      <c r="AD45" s="96"/>
-      <c r="AE45" s="96"/>
+      <c r="AD45" s="95"/>
+      <c r="AE45" s="95"/>
       <c r="AF45" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="AG45" s="107"/>
+      <c r="AG45" s="97"/>
     </row>
-    <row r="46" spans="1:33" s="97" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="93">
-        <f t="shared" si="2"/>
+    <row r="46" spans="1:33" s="96" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="108">
         <v>44</v>
       </c>
       <c r="B46" s="88"/>
@@ -7939,49 +7881,48 @@
       <c r="L46" s="87"/>
       <c r="M46" s="87"/>
       <c r="N46" s="87"/>
-      <c r="O46" s="94"/>
+      <c r="O46" s="93"/>
       <c r="P46" s="87"/>
       <c r="Q46" s="87"/>
-      <c r="R46" s="95">
+      <c r="R46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="S46" s="87"/>
-      <c r="T46" s="95">
+      <c r="T46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="U46" s="87"/>
-      <c r="V46" s="95">
+      <c r="V46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
       <c r="W46" s="87"/>
-      <c r="X46" s="95">
+      <c r="X46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
       <c r="Y46" s="87"/>
-      <c r="Z46" s="95">
+      <c r="Z46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AA46" s="87"/>
-      <c r="AB46" s="95">
+      <c r="AB46" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC46" s="87"/>
-      <c r="AD46" s="96"/>
-      <c r="AE46" s="96"/>
+      <c r="AD46" s="95"/>
+      <c r="AE46" s="95"/>
       <c r="AF46" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="AG46" s="107"/>
+      <c r="AG46" s="97"/>
     </row>
-    <row r="47" spans="1:33" s="97" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="93">
-        <f t="shared" si="2"/>
+    <row r="47" spans="1:33" s="96" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="108">
         <v>45</v>
       </c>
       <c r="B47" s="88"/>
@@ -8007,49 +7948,48 @@
       <c r="L47" s="87"/>
       <c r="M47" s="87"/>
       <c r="N47" s="87"/>
-      <c r="O47" s="94"/>
+      <c r="O47" s="93"/>
       <c r="P47" s="87"/>
       <c r="Q47" s="87"/>
-      <c r="R47" s="95">
+      <c r="R47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="S47" s="87"/>
-      <c r="T47" s="95">
+      <c r="T47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
       <c r="U47" s="87"/>
-      <c r="V47" s="95">
+      <c r="V47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
       <c r="W47" s="87"/>
-      <c r="X47" s="95">
+      <c r="X47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
       <c r="Y47" s="87"/>
-      <c r="Z47" s="95">
+      <c r="Z47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AA47" s="87"/>
-      <c r="AB47" s="95">
+      <c r="AB47" s="94">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC47" s="87"/>
-      <c r="AD47" s="96"/>
-      <c r="AE47" s="96"/>
+      <c r="AD47" s="95"/>
+      <c r="AE47" s="95"/>
       <c r="AF47" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="AG47" s="107"/>
+      <c r="AG47" s="97"/>
     </row>
     <row r="48" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="33">
-        <f t="shared" si="2"/>
+      <c r="A48" s="108">
         <v>46</v>
       </c>
       <c r="B48" s="80">
@@ -8125,18 +8065,16 @@
       <c r="AD48" s="92"/>
       <c r="AE48" s="92"/>
       <c r="AF48" s="15"/>
-      <c r="AG48" s="107"/>
+      <c r="AG48" s="97"/>
     </row>
     <row r="49" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="33">
-        <f t="shared" si="2"/>
+      <c r="A49" s="108">
         <v>47</v>
       </c>
       <c r="B49" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C49" s="90">
-        <f>C48+0.001</f>
         <v>2.2749999999999999</v>
       </c>
       <c r="D49" s="63" t="s">
@@ -8206,18 +8144,16 @@
       <c r="AD49" s="92"/>
       <c r="AE49" s="92"/>
       <c r="AF49" s="15"/>
-      <c r="AG49" s="107"/>
+      <c r="AG49" s="97"/>
     </row>
     <row r="50" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="33">
-        <f t="shared" si="2"/>
+      <c r="A50" s="108">
         <v>48</v>
       </c>
       <c r="B50" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C50" s="90">
-        <f t="shared" ref="C50:C58" si="4">C49+0.001</f>
         <v>2.2759999999999998</v>
       </c>
       <c r="D50" s="63" t="s">
@@ -8287,18 +8223,16 @@
       <c r="AD50" s="92"/>
       <c r="AE50" s="92"/>
       <c r="AF50" s="15"/>
-      <c r="AG50" s="107"/>
+      <c r="AG50" s="97"/>
     </row>
     <row r="51" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="33">
-        <f t="shared" si="2"/>
+      <c r="A51" s="108">
         <v>49</v>
       </c>
       <c r="B51" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C51" s="90">
-        <f t="shared" si="4"/>
         <v>2.2769999999999997</v>
       </c>
       <c r="D51" s="63" t="s">
@@ -8368,18 +8302,16 @@
       <c r="AD51" s="92"/>
       <c r="AE51" s="92"/>
       <c r="AF51" s="15"/>
-      <c r="AG51" s="107"/>
+      <c r="AG51" s="97"/>
     </row>
     <row r="52" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="33">
-        <f t="shared" si="2"/>
+      <c r="A52" s="108">
         <v>50</v>
       </c>
       <c r="B52" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C52" s="90">
-        <f t="shared" si="4"/>
         <v>2.2779999999999996</v>
       </c>
       <c r="D52" s="63" t="s">
@@ -8449,18 +8381,16 @@
       <c r="AD52" s="92"/>
       <c r="AE52" s="92"/>
       <c r="AF52" s="15"/>
-      <c r="AG52" s="107"/>
+      <c r="AG52" s="97"/>
     </row>
     <row r="53" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="33">
-        <f t="shared" si="2"/>
+      <c r="A53" s="108">
         <v>51</v>
       </c>
       <c r="B53" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C53" s="90">
-        <f t="shared" si="4"/>
         <v>2.2789999999999995</v>
       </c>
       <c r="D53" s="63" t="s">
@@ -8530,18 +8460,16 @@
       <c r="AD53" s="92"/>
       <c r="AE53" s="92"/>
       <c r="AF53" s="15"/>
-      <c r="AG53" s="107"/>
+      <c r="AG53" s="97"/>
     </row>
     <row r="54" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="33">
-        <f t="shared" si="2"/>
+      <c r="A54" s="108">
         <v>52</v>
       </c>
       <c r="B54" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C54" s="90">
-        <f t="shared" si="4"/>
         <v>2.2799999999999994</v>
       </c>
       <c r="D54" s="63" t="s">
@@ -8611,18 +8539,16 @@
       <c r="AD54" s="92"/>
       <c r="AE54" s="92"/>
       <c r="AF54" s="15"/>
-      <c r="AG54" s="107"/>
+      <c r="AG54" s="97"/>
     </row>
     <row r="55" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="33">
-        <f t="shared" si="2"/>
+      <c r="A55" s="108">
         <v>53</v>
       </c>
       <c r="B55" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C55" s="90">
-        <f t="shared" si="4"/>
         <v>2.2809999999999993</v>
       </c>
       <c r="D55" s="63" t="s">
@@ -8692,18 +8618,16 @@
       <c r="AD55" s="92"/>
       <c r="AE55" s="92"/>
       <c r="AF55" s="15"/>
-      <c r="AG55" s="107"/>
+      <c r="AG55" s="97"/>
     </row>
     <row r="56" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="33">
-        <f t="shared" si="2"/>
+      <c r="A56" s="108">
         <v>54</v>
       </c>
       <c r="B56" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C56" s="90">
-        <f t="shared" si="4"/>
         <v>2.2819999999999991</v>
       </c>
       <c r="D56" s="63" t="s">
@@ -8773,18 +8697,16 @@
       <c r="AD56" s="92"/>
       <c r="AE56" s="92"/>
       <c r="AF56" s="15"/>
-      <c r="AG56" s="107"/>
+      <c r="AG56" s="97"/>
     </row>
     <row r="57" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="33">
-        <f t="shared" si="2"/>
+      <c r="A57" s="108">
         <v>55</v>
       </c>
       <c r="B57" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C57" s="90">
-        <f t="shared" si="4"/>
         <v>2.282999999999999</v>
       </c>
       <c r="D57" s="63" t="s">
@@ -8854,18 +8776,16 @@
       <c r="AD57" s="92"/>
       <c r="AE57" s="92"/>
       <c r="AF57" s="15"/>
-      <c r="AG57" s="107"/>
+      <c r="AG57" s="97"/>
     </row>
     <row r="58" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="33">
-        <f t="shared" si="2"/>
+      <c r="A58" s="108">
         <v>56</v>
       </c>
       <c r="B58" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C58" s="90">
-        <f t="shared" si="4"/>
         <v>2.2839999999999989</v>
       </c>
       <c r="D58" s="63" t="s">
@@ -8935,18 +8855,16 @@
       <c r="AD58" s="92"/>
       <c r="AE58" s="92"/>
       <c r="AF58" s="15"/>
-      <c r="AG58" s="107"/>
+      <c r="AG58" s="97"/>
     </row>
     <row r="59" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="33">
-        <f t="shared" si="2"/>
+      <c r="A59" s="108">
         <v>57</v>
       </c>
       <c r="B59" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C59" s="90">
-        <f>C58+0.002</f>
         <v>2.2859999999999987</v>
       </c>
       <c r="D59" s="63" t="s">
@@ -9016,18 +8934,16 @@
       <c r="AD59" s="92"/>
       <c r="AE59" s="92"/>
       <c r="AF59" s="15"/>
-      <c r="AG59" s="107"/>
+      <c r="AG59" s="97"/>
     </row>
     <row r="60" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="33">
-        <f t="shared" si="2"/>
+      <c r="A60" s="109">
         <v>58</v>
       </c>
       <c r="B60" s="80">
         <v>2.7669999999999999</v>
       </c>
       <c r="C60" s="90">
-        <f>C59+0.001</f>
         <v>2.2869999999999986</v>
       </c>
       <c r="D60" s="63" t="s">
@@ -9097,7 +9013,7 @@
       <c r="AD60" s="92"/>
       <c r="AE60" s="92"/>
       <c r="AF60" s="15"/>
-      <c r="AG60" s="107"/>
+      <c r="AG60" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -9245,7 +9161,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>55</v>

</xml_diff>